<commit_message>
Adding Process workflow and finalize the project
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oumaima.moulay.taj\Documents\UiPath\Amazon_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2E8CD9-C57C-420F-8C3E-761D97DE6C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C4F425-DA4C-4D2B-AC66-E5037FC8E8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>Amazon_WebSite</t>
   </si>
   <si>
     <t>Amazon_REF</t>
@@ -563,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -614,7 +611,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -625,7 +622,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -637,7 +634,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -646,10 +643,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -658,13 +655,13 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>10000</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1840,7 +1837,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>41</v>
@@ -2827,8 +2824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2876,15 +2873,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>